<commit_message>
direct parsing from md via txt, bugfixes for encoding
</commit_message>
<xml_diff>
--- a/output/cpc03-CG-md.xlsx
+++ b/output/cpc03-CG-md.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="67">
   <si>
     <t>PARAGRAPH NUMBER</t>
   </si>
@@ -55,7 +55,7 @@
     <t>shell radius</t>
   </si>
   <si>
-    <t>15</t>
+    <t>15 Å</t>
   </si>
   <si>
     <t>ions</t>
@@ -106,7 +106,7 @@
     <t>cut</t>
   </si>
   <si>
-    <t>9</t>
+    <t>9 Å</t>
   </si>
   <si>
     <t>period</t>
@@ -166,7 +166,7 @@
     <t>restraint_wt</t>
   </si>
   <si>
-    <t>25</t>
+    <t>25 kcal mol-1 Å-2</t>
   </si>
   <si>
     <t>Thermalization</t>
@@ -202,7 +202,7 @@
     <t>10</t>
   </si>
   <si>
-    <t>0</t>
+    <t>0 kcal mol-1 Å-2</t>
   </si>
   <si>
     <t>250</t>
@@ -212,6 +212,9 @@
   </si>
   <si>
     <t>overall repetitions</t>
+  </si>
+  <si>
+    <t>1 µs</t>
   </si>
 </sst>
 </file>
@@ -1052,7 +1055,7 @@
         <v>52</v>
       </c>
       <c r="C46" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add image extraction functionality for MD-based document
</commit_message>
<xml_diff>
--- a/output/cpc03-CG-md.xlsx
+++ b/output/cpc03-CG-md.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="70">
   <si>
     <t>PARAGRAPH NUMBER</t>
   </si>
@@ -100,7 +100,7 @@
     <t>dt</t>
   </si>
   <si>
-    <t>2</t>
+    <t>2 fs</t>
   </si>
   <si>
     <t>cut</t>
@@ -115,10 +115,10 @@
     <t>production</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>8</t>
+    <t>4 fs</t>
+  </si>
+  <si>
+    <t>8 Å</t>
   </si>
   <si>
     <t>step type</t>
@@ -166,7 +166,7 @@
     <t>restraint_wt</t>
   </si>
   <si>
-    <t>25 kcal mol-1 Å-2</t>
+    <t>25 kcal mol-1 Å^-2^</t>
   </si>
   <si>
     <t>Thermalization</t>
@@ -175,7 +175,7 @@
     <t>simulation time</t>
   </si>
   <si>
-    <t>50</t>
+    <t>50 ps</t>
   </si>
   <si>
     <t>MD</t>
@@ -190,28 +190,37 @@
     <t>100 K</t>
   </si>
   <si>
-    <t>300</t>
+    <t>300 ps</t>
   </si>
   <si>
     <t>pres0</t>
   </si>
   <si>
-    <t>1</t>
+    <t>1 atm</t>
+  </si>
+  <si>
+    <t>300 K</t>
+  </si>
+  <si>
+    <t>10 kcal mol^-1^ Å^-2^</t>
+  </si>
+  <si>
+    <t>300 ns</t>
+  </si>
+  <si>
+    <t>0 kcal mol^-1^ Å^-2^</t>
+  </si>
+  <si>
+    <t>250 ns</t>
+  </si>
+  <si>
+    <t>Production</t>
+  </si>
+  <si>
+    <t>overall repetitions</t>
   </si>
   <si>
     <t>10</t>
-  </si>
-  <si>
-    <t>0 kcal mol-1 Å-2</t>
-  </si>
-  <si>
-    <t>250</t>
-  </si>
-  <si>
-    <t>Production</t>
-  </si>
-  <si>
-    <t>overall repetitions</t>
   </si>
   <si>
     <t>1 µs</t>
@@ -956,7 +965,7 @@
         <v>56</v>
       </c>
       <c r="C37" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -967,7 +976,7 @@
         <v>49</v>
       </c>
       <c r="C38" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -978,7 +987,7 @@
         <v>52</v>
       </c>
       <c r="C39" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1000,7 +1009,7 @@
         <v>49</v>
       </c>
       <c r="C41" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1011,7 +1020,7 @@
         <v>52</v>
       </c>
       <c r="C42" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1022,7 +1031,7 @@
         <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1030,10 +1039,10 @@
         <v>16</v>
       </c>
       <c r="B44" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C44" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1055,7 +1064,7 @@
         <v>52</v>
       </c>
       <c r="C46" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>